<commit_message>
Read the cellData from Excel and show in console - ready Read the columnData from Excel and show in console - ready Creating ArrayList from Excel - ready Multiplication ArrayList<Integer> by Int - ready
ArrayList<Cell> to ArrayList<Integer> - not ready.
</commit_message>
<xml_diff>
--- a/src/main/DataSource/ArrayData1.xlsx
+++ b/src/main/DataSource/ArrayData1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218D0366-3307-4CF6-9C4C-E7CDD66A44AD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BEDF4AF-3D8F-4EA9-A922-02F2E6418959}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5460" yWindow="696" windowWidth="15852" windowHeight="11664" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -418,7 +418,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -558,9 +558,7 @@
       <c r="C8" s="1">
         <v>5</v>
       </c>
-      <c r="D8" s="1">
-        <v>40</v>
-      </c>
+      <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
ArrayListCellFromExcel - создает ArrayList<Cell>
ArrayListIntFromExcel - не ArrayList<Integer>,ошибка?

package GetExcelData - пакет с классами для чтения Эксель.
папка DataSource - Эксель файл из которого считываются данные.
</commit_message>
<xml_diff>
--- a/src/main/DataSource/ArrayData1.xlsx
+++ b/src/main/DataSource/ArrayData1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BEDF4AF-3D8F-4EA9-A922-02F2E6418959}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FD1512-8CDF-4CD2-930F-279AE8F671E8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5460" yWindow="696" windowWidth="15852" windowHeight="11664" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -418,7 +418,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -467,9 +467,7 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
-        <v>7</v>
-      </c>
+      <c r="B3" s="1"/>
       <c r="C3" s="1">
         <v>35</v>
       </c>
@@ -490,9 +488,7 @@
       <c r="C4" s="1">
         <v>1000</v>
       </c>
-      <c r="D4" s="1">
-        <v>45</v>
-      </c>
+      <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
         <v>13</v>
       </c>
@@ -504,9 +500,7 @@
       <c r="B5" s="1">
         <v>100</v>
       </c>
-      <c r="C5" s="1">
-        <v>1000</v>
-      </c>
+      <c r="C5" s="1"/>
       <c r="D5" s="1">
         <v>555</v>
       </c>
@@ -518,9 +512,7 @@
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
+      <c r="B6" s="1"/>
       <c r="C6" s="1">
         <v>11</v>
       </c>
@@ -567,9 +559,7 @@
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1">
-        <v>25750</v>
-      </c>
+      <c r="B9" s="1"/>
       <c r="C9" s="1">
         <v>5</v>
       </c>

</xml_diff>